<commit_message>
OpenTBS updates, with doc and demo
</commit_message>
<xml_diff>
--- a/demo/demo_ms_excel.xlsx
+++ b/demo/demo_ms_excel.xlsx
@@ -63,28 +63,28 @@
     <t xml:space="preserve">   For example: writing [b1.title;block=row] in the template, and calling $TBS-&gt;MergeBlock('b1', ...) will produce an error because there is no &lt;row&gt; tag in the SharedStrings subfile.</t>
   </si>
   <si>
-    <t>Merging Microsoft Excel templates with OpenTBS has several big limitations because of the OpenXML format they are saved under.</t>
-  </si>
-  <si>
     <t>OpenTBS demo</t>
   </si>
   <si>
     <t>You can anly use simple TBS fields. Which is quite few.</t>
   </si>
   <si>
-    <t>* Texts in cells are not saved in the sheet subfile but in the 'xl/sharedStrings.xml' subfile. This means you cannot refer to any sheet tags for TBS tags placed in a text cell.</t>
-  </si>
-  <si>
-    <t>Far all those raisons, its seems than it is not possible to use MergeBlock() nore OpenXML tags in an Excel template for OpenTBS :-(</t>
-  </si>
-  <si>
-    <t>* Formulas are saved in the sheets subfile with both the expression and the result. This means that when you write one TBS tag in the template, it may have two in the XML subfile.</t>
-  </si>
-  <si>
-    <t>* Pictures placed in the sheet are not saved in the sheet subfile but in another XML subfile (for instance 'xl\drawings\drawing1.xml'). This means you cannot use the usual parameter "ope=changepic" to change pictures in a sheet.</t>
-  </si>
-  <si>
-    <t>* Cells are saved in sheets with their absolute position (row, column). Thus, when you merge them using MergeBlock(), positions are duplicated. This can produce wrong sheets.</t>
+    <t>Merging Microsoft Excel templates with OpenTBS has several big limitations because of the OpenXML format for Excel.</t>
+  </si>
+  <si>
+    <t>* Excel formulas are saved in Sheet subfiles with both the expression and the result. This means that when you write one TBS tag in Excel, it may have two in the XML source of the template.</t>
+  </si>
+  <si>
+    <t>* Texts in cells are not saved in the sheet subfile but in the 'xl/sharedStrings.xml' subfile. This means you cannot refer to any sheet tag (like row) for TBS tags placed in a text cell.</t>
+  </si>
+  <si>
+    <t>* Pictures placed in the sheet are not referenced in the sheet subfile but in another XML subfile (for instance 'xl\drawings\drawing1.xml'). This means you cannot use the usual parameter "ope=changepic" to change pictures in a sheet.</t>
+  </si>
+  <si>
+    <t>* Cells are saved in sheets with their absolute position (row+column). Thus, when you merge them using MergeBlock(), positions are duplicated. This can produce wrong sheets.</t>
+  </si>
+  <si>
+    <t>Far all those raisons, its seems than it is not possible to use MergeBlock() an Excel template.</t>
   </si>
 </sst>
 </file>
@@ -461,7 +461,7 @@
   <dimension ref="B2:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -471,7 +471,7 @@
   <sheetData>
     <row r="2" spans="2:2" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
@@ -506,17 +506,17 @@
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="2:2" x14ac:dyDescent="0.25">
@@ -526,22 +526,22 @@
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Merging Excel sheets is now possible
</commit_message>
<xml_diff>
--- a/demo/demo_ms_excel.xlsx
+++ b/demo/demo_ms_excel.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Nothing here.</t>
   </si>
@@ -57,34 +57,43 @@
     <t>This is a demo of the OpenTBS plugin.</t>
   </si>
   <si>
+    <t>OpenTBS demo</t>
+  </si>
+  <si>
+    <t>Example #1: merging data with rows</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Membership number</t>
+  </si>
+  <si>
+    <t>[a.name]</t>
+  </si>
+  <si>
+    <t>[a.number]</t>
+  </si>
+  <si>
+    <t>[a.firstname;block=row]</t>
+  </si>
+  <si>
     <t>You may consider the following before building your own Microsoft Excel template:</t>
   </si>
   <si>
-    <t xml:space="preserve">   For example: writing [b1.title;block=row] in the template, and calling $TBS-&gt;MergeBlock('b1', ...) will produce an error because there is no &lt;row&gt; tag in the SharedStrings subfile.</t>
-  </si>
-  <si>
-    <t>OpenTBS demo</t>
-  </si>
-  <si>
-    <t>You can anly use simple TBS fields. Which is quite few.</t>
-  </si>
-  <si>
-    <t>Merging Microsoft Excel templates with OpenTBS has several big limitations because of the OpenXML format for Excel.</t>
-  </si>
-  <si>
-    <t>* Excel formulas are saved in Sheet subfiles with both the expression and the result. This means that when you write one TBS tag in Excel, it may have two in the XML source of the template.</t>
-  </si>
-  <si>
-    <t>* Texts in cells are not saved in the sheet subfile but in the 'xl/sharedStrings.xml' subfile. This means you cannot refer to any sheet tag (like row) for TBS tags placed in a text cell.</t>
-  </si>
-  <si>
-    <t>* Pictures placed in the sheet are not referenced in the sheet subfile but in another XML subfile (for instance 'xl\drawings\drawing1.xml'). This means you cannot use the usual parameter "ope=changepic" to change pictures in a sheet.</t>
-  </si>
-  <si>
-    <t>* Cells are saved in sheets with their absolute position (row+column). Thus, when you merge them using MergeBlock(), positions are duplicated. This can produce wrong sheets.</t>
-  </si>
-  <si>
-    <t>Far all those raisons, its seems than it is not possible to use MergeBlock() an Excel template.</t>
+    <t>Merging Microsoft Excel templates with OpenTBS has several limitations because of the OpenXML format for Excel.</t>
+  </si>
+  <si>
+    <t>* Formulas won't work because OpenTBS needs to convert cell positions from aboslute to relative in order to have a constistent merged sheet.</t>
+  </si>
+  <si>
+    <t>* Formulas may also make troubles because they are saved twice in the sheet:  one for the expression, and one for the instant result.</t>
+  </si>
+  <si>
+    <t>* Changing picture (using ope=changepic)  because drawing information are saved in another XML sub-file.</t>
   </si>
 </sst>
 </file>
@@ -112,12 +121,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color indexed="16"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="16"/>
       <color indexed="8"/>
@@ -127,20 +130,35 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color indexed="16"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -148,13 +166,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -458,20 +493,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:B21"/>
+  <dimension ref="B2:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.140625" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:2" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B2" s="2" t="s">
-        <v>8</v>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
@@ -500,54 +538,61 @@
       </c>
     </row>
     <row r="12" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B12" s="3" t="s">
-        <v>6</v>
+      <c r="B12" s="5" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B14" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B15" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B16" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
+      <c r="D21" s="3" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B16" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
OpenTBS: enhanced Excel example
</commit_message>
<xml_diff>
--- a/demo/demo_ms_excel.xlsx
+++ b/demo/demo_ms_excel.xlsx
@@ -10,12 +10,12 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="114210"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Nothing here.</t>
   </si>
@@ -129,22 +129,35 @@
     <t>[onshow.x_num;ope=xlsxNum]</t>
   </si>
   <si>
-    <t>* Do not use a formula in a cell that may have its position changed after the merge (for example under TBS block). Otherwise Excel will raise an error message.</t>
-  </si>
-  <si>
     <t>* You cannot change picture using "ope=changepic". This is because drawing information are not saved directly in the sheet.</t>
   </si>
   <si>
     <t xml:space="preserve">* If a formula uses a reference to a cell that has moved during the merge, then the reference will not be arraged to be the new cell reference. </t>
+  </si>
+  <si>
+    <t>* Do not use a formula in a cell that may have its position changed after the merge (for example under a TBS block). Otherwise Excel will raise an error message.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    This is because the location of formulas are saved a second time in another sub-file for the order of evaluation.</t>
+  </si>
+  <si>
+    <t>Score</t>
+  </si>
+  <si>
+    <t>[a.score;ope=xlsxNum]</t>
+  </si>
+  <si>
+    <t>Total:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#,##0.0000"/>
     <numFmt numFmtId="165" formatCode="dd\ mmmm\ yyyy"/>
+    <numFmt numFmtId="167" formatCode="#,##0.0"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -239,7 +252,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -249,6 +262,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -550,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D30"/>
+  <dimension ref="B2:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,12 +621,12 @@
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.25">
@@ -614,89 +634,109 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="4" t="s">
+    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B16" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="2" t="s">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D19" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" s="10">
+        <f>SUM(E21:E2000)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="3" t="s">
+      <c r="E20" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C21" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D21" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="4" t="s">
+      <c r="E21" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="5" t="s">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="5" t="s">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="6" t="s">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C28" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D28" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
         <v>19</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C29" t="s">
         <v>22</v>
       </c>
-      <c r="D28" s="7" t="s">
+      <c r="D29" s="7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
         <v>20</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C30" t="s">
         <v>23</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D30" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
         <v>21</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C31" t="s">
         <v>25</v>
       </c>
-      <c r="D30" s="8" t="s">
+      <c r="D31" s="8" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
OpenTBS: fix a bug
</commit_message>
<xml_diff>
--- a/demo/demo_ms_excel.xlsx
+++ b/demo/demo_ms_excel.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <t>Nothing here.</t>
   </si>
@@ -84,9 +84,6 @@
     <t>You may consider the following before building your own Microsoft Excel template:</t>
   </si>
   <si>
-    <t>Exampe #2: change the type data in a cell</t>
-  </si>
-  <si>
     <t>Type of data</t>
   </si>
   <si>
@@ -148,6 +145,21 @@
   </si>
   <si>
     <t>Total:</t>
+  </si>
+  <si>
+    <t>Example #2: merging data with columns</t>
+  </si>
+  <si>
+    <t>First Name:</t>
+  </si>
+  <si>
+    <t>[b1.firstname;block=c]</t>
+  </si>
+  <si>
+    <t>[b2.score;block=c;ope=xlsxNum]</t>
+  </si>
+  <si>
+    <t>Example #3: change the type data in a cell</t>
   </si>
 </sst>
 </file>
@@ -157,7 +169,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#,##0.0000"/>
     <numFmt numFmtId="165" formatCode="dd\ mmmm\ yyyy"/>
-    <numFmt numFmtId="167" formatCode="#,##0.0"/>
+    <numFmt numFmtId="166" formatCode="#,##0.0"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -252,7 +264,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -265,9 +277,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -570,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E31"/>
+  <dimension ref="B2:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -589,11 +607,13 @@
         <v>6</v>
       </c>
     </row>
+    <row r="3" spans="2:2" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
     </row>
+    <row r="5" spans="2:2" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>5</v>
@@ -604,19 +624,24 @@
         <v>4</v>
       </c>
     </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+    </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.25">
@@ -626,118 +651,134 @@
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B16" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="4" t="s">
-        <v>7</v>
+      <c r="D18" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="10">
+        <f>SUM(E20:E2004)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D19" s="9" t="s">
+      <c r="B19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E19" s="10">
-        <f>SUM(E21:E2000)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E21" s="11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="4" t="s">
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="5" t="s">
+      <c r="C32" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>18</v>
+      </c>
+      <c r="C33" t="s">
+        <v>21</v>
+      </c>
+      <c r="D33" s="7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
         <v>19</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C34" t="s">
         <v>22</v>
       </c>
-      <c r="D29" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
+      <c r="D34" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
         <v>20</v>
       </c>
-      <c r="C30" t="s">
-        <v>23</v>
-      </c>
-      <c r="D30" t="s">
+      <c r="C35" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>21</v>
-      </c>
-      <c r="C31" t="s">
+      <c r="D35" s="8" t="s">
         <v>25</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
OpenTBS 1.6.1 better templates
</commit_message>
<xml_diff>
--- a/demo/demo_ms_excel.xlsx
+++ b/demo/demo_ms_excel.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="49">
   <si>
     <t>PHP version : [onshow..cst.PHP_VERSION]</t>
   </si>
@@ -181,6 +181,9 @@
   </si>
   <si>
     <t>of the table for those fields are created dynamically in the sheet.</t>
+  </si>
+  <si>
+    <t>Example #1-bis: chart based on dynamic contents</t>
   </si>
 </sst>
 </file>
@@ -328,6 +331,160 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Score of the team</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Examples part 1'!$C$20:$C$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>[a.name]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Examples part 1'!$E$20:$E$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0" formatCode="#,##0.0">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="28864896"/>
+        <c:axId val="29424640"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="28864896"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="29424640"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="29424640"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="#,##0.0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="28864896"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>19049</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>752475</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -617,7 +774,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E35"/>
+  <dimension ref="B2:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
@@ -688,12 +845,15 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="H17" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D18" s="9" t="s">
         <v>34</v>
       </c>
@@ -702,7 +862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
         <v>7</v>
       </c>
@@ -716,7 +876,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
         <v>12</v>
       </c>
@@ -730,12 +890,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
         <v>35</v>
       </c>
@@ -743,7 +903,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
         <v>32</v>
       </c>
@@ -751,22 +911,22 @@
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B32" s="6" t="s">
         <v>14</v>
       </c>
@@ -814,6 +974,7 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
OpenTBS: demo, manual, and few renaming
</commit_message>
<xml_diff>
--- a/demo/demo_ms_excel.xlsx
+++ b/demo/demo_ms_excel.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="45" windowWidth="17400" windowHeight="11955"/>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="57">
   <si>
     <t>PHP version : [onshow..cst.PHP_VERSION]</t>
   </si>
@@ -303,6 +303,21 @@
       <t>:</t>
     </r>
   </si>
+  <si>
+    <t>Example #5: pictures in Ms Excel</t>
+  </si>
+  <si>
+    <t>command OPENTBS_MERGE_SPECIAL_ITEMS at the PHP side.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In Ms Excel, pictures are not actually saved in the sheet. </t>
+  </si>
+  <si>
+    <t>Therefore, in order to change the picture you have to put the TBS fields inside</t>
+  </si>
+  <si>
+    <t>the description (or title) of the picture item, and use</t>
+  </si>
 </sst>
 </file>
 
@@ -313,7 +328,7 @@
     <numFmt numFmtId="165" formatCode="dd\ mmmm\ yyyy"/>
     <numFmt numFmtId="166" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -385,6 +400,14 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -412,7 +435,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -435,16 +458,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -468,9 +500,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Titre 3" xfId="1" builtinId="18"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -550,11 +584,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="81080704"/>
-        <c:axId val="81082240"/>
+        <c:axId val="45896064"/>
+        <c:axId val="45897600"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="81080704"/>
+        <c:axId val="45896064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -563,7 +597,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81082240"/>
+        <c:crossAx val="45897600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -571,7 +605,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="81082240"/>
+        <c:axId val="45897600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -582,7 +616,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81080704"/>
+        <c:crossAx val="45896064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -634,6 +668,55 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>914400</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>663833</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>149569</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1" descr="[onshow.x_picture;ope=changepic;tagpos=inside]"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5543550" y="2847975"/>
+          <a:ext cx="1130558" cy="1511644"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -971,44 +1054,44 @@
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="12" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="4" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="4" t="s">
+    <row r="17" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="H17" s="4" t="s">
+      <c r="H17" s="17" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D18" s="14"/>
-      <c r="E18" s="15" t="s">
+      <c r="D18" s="13"/>
+      <c r="E18" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="F18" s="16">
+      <c r="F18" s="15">
         <f>SUM(F20:F2005)</f>
         <v>0</v>
       </c>
@@ -1040,25 +1123,25 @@
       <c r="D20" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E20" s="9" t="s">
+      <c r="E20" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="F20" s="9" t="s">
+      <c r="F20" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C21" s="14"/>
-      <c r="D21" s="17" t="s">
+      <c r="C21" s="13"/>
+      <c r="D21" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="E21" s="16">
-        <f ca="1">SUM( E20   : INDIRECT(ADDRESS(ROW()-1,COLUMN())) )</f>
+      <c r="E21" s="15">
+        <f ca="1">SUM( E20    : INDIRECT(ADDRESS(ROW()-1,COLUMN())) )</f>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="4" t="s">
+    <row r="23" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="17" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1066,7 +1149,7 @@
       <c r="B25" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C25" s="9" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1074,33 +1157,33 @@
       <c r="B26" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="C26" s="10" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="4" t="s">
+    <row r="28" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="17" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="4" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="5" t="s">
+      <c r="B31" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C33" s="6" t="s">
+      <c r="C33" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D33" s="6" t="s">
+      <c r="D33" s="5" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1111,7 +1194,7 @@
       <c r="C34" t="s">
         <v>20</v>
       </c>
-      <c r="D34" s="7" t="s">
+      <c r="D34" s="6" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1133,7 +1216,7 @@
       <c r="C36" t="s">
         <v>23</v>
       </c>
-      <c r="D36" s="8" t="s">
+      <c r="D36" s="7" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1148,10 +1231,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D9"/>
+  <dimension ref="B2:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1160,23 +1243,23 @@
     <col min="4" max="6" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="17" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1187,7 +1270,7 @@
       <c r="C8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="12" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1198,14 +1281,40 @@
       <c r="C9" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="11" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="17" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="4" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
OpenTBS : update examples
</commit_message>
<xml_diff>
--- a/demo/demo_ms_excel.xlsx
+++ b/demo/demo_ms_excel.xlsx
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="58">
   <si>
     <t>PHP version : [onshow..cst.PHP_VERSION]</t>
   </si>
@@ -120,9 +120,6 @@
     <t>OpenTBS demo</t>
   </si>
   <si>
-    <t>Example #1: merging data with rows</t>
-  </si>
-  <si>
     <t>First Name</t>
   </si>
   <si>
@@ -204,12 +201,6 @@
     <t>First Name:</t>
   </si>
   <si>
-    <t>Example #3: change the type data in a cell</t>
-  </si>
-  <si>
-    <t>Example #2: merging data with cell (extending columns)</t>
-  </si>
-  <si>
     <t>[cell1.firstname;block=c]</t>
   </si>
   <si>
@@ -219,9 +210,6 @@
     <t>[b2.name]</t>
   </si>
   <si>
-    <t>Example #4: dynamic columns</t>
-  </si>
-  <si>
     <t>In the example below, the data already contains fields « email_1 », « email_2 » and « email_3 », but the columns</t>
   </si>
   <si>
@@ -229,9 +217,6 @@
   </si>
   <si>
     <t>of the table for those fields are created dynamically in the sheet.</t>
-  </si>
-  <si>
-    <t>Example #1-bis: chart based on dynamic contents</t>
   </si>
   <si>
     <t>This sheet will be deleted.</t>
@@ -292,9 +277,6 @@
     </r>
   </si>
   <si>
-    <t>Example #5: pictures in Ms Excel</t>
-  </si>
-  <si>
     <t>command OPENTBS_MERGE_SPECIAL_ITEMS at the PHP side.</t>
   </si>
   <si>
@@ -317,6 +299,27 @@
   </si>
   <si>
     <t>Email [cell1.val;block=tbs:cell]</t>
+  </si>
+  <si>
+    <t>Merging data with rows</t>
+  </si>
+  <si>
+    <t>Merging data with cell (extending columns)</t>
+  </si>
+  <si>
+    <t>Change the type data in a cell</t>
+  </si>
+  <si>
+    <t>Chart based on dynamic contents</t>
+  </si>
+  <si>
+    <t>Dynamic columns</t>
+  </si>
+  <si>
+    <t>Pictures in Ms Excel</t>
+  </si>
+  <si>
+    <t>Delete a sheet</t>
   </si>
 </sst>
 </file>
@@ -328,7 +331,7 @@
     <numFmt numFmtId="165" formatCode="dd\ mmmm\ yyyy"/>
     <numFmt numFmtId="166" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -407,6 +410,14 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FF4F81BD"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="5">
@@ -500,7 +511,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -508,6 +519,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF4F81BD"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -584,11 +600,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="82329984"/>
-        <c:axId val="82331520"/>
+        <c:axId val="54892800"/>
+        <c:axId val="80426112"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="82329984"/>
+        <c:axId val="54892800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -597,7 +613,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82331520"/>
+        <c:crossAx val="80426112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -605,7 +621,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82331520"/>
+        <c:axId val="80426112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -616,7 +632,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82329984"/>
+        <c:crossAx val="54892800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -686,7 +702,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>663833</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>149569</xdr:rowOff>
+      <xdr:rowOff>140044</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1055,41 +1071,41 @@
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B17" s="17" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="H17" s="17" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D18" s="13"/>
       <c r="E18" s="14" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F18" s="15">
         <f>SUM(F20:F2005)</f>
@@ -1098,126 +1114,126 @@
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="E19" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C20" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="E20" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C21" s="13"/>
       <c r="D21" s="16" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E21" s="15">
-        <f ca="1">SUM( E20      : INDIRECT(ADDRESS(ROW()-1,COLUMN())) )</f>
+        <f ca="1">SUM( E20       : INDIRECT(ADDRESS(ROW()-1,COLUMN())) )</f>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:8" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B23" s="17" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="9" t="s">
         <v>33</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B28" s="17" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="D33" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C34" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C35" t="s">
+        <v>19</v>
+      </c>
+      <c r="D35" t="s">
         <v>20</v>
-      </c>
-      <c r="D35" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C36" t="s">
+        <v>21</v>
+      </c>
+      <c r="D36" s="7" t="s">
         <v>22</v>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1231,7 +1247,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D20"/>
+  <dimension ref="B2:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1241,71 +1257,71 @@
     <col min="4" max="6" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B2" s="17" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="D8" s="12" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B16" s="17" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="4" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="4" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1329,7 +1345,7 @@
   <sheetData>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1339,15 +1355,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3"/>
+  <dimension ref="B2:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>44</v>
+    <row r="2" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B2" s="17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
OpenTbs 1.8.1 beta - new common keywords for changing cell types in ODS and XLSX.
</commit_message>
<xml_diff>
--- a/demo/demo_ms_excel.xlsx
+++ b/demo/demo_ms_excel.xlsx
@@ -12,6 +12,9 @@
     <sheet name="Display me" sheetId="4" state="hidden" r:id="rId3"/>
     <sheet name="Delete me" sheetId="3" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="the_named_cell">'Delete me'!$B$6</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
@@ -78,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="60">
   <si>
     <t>PHP version : [onshow..cst.PHP_VERSION]</t>
   </si>
@@ -156,30 +159,12 @@
     <t>Date/time</t>
   </si>
   <si>
-    <t>xlsxNum</t>
-  </si>
-  <si>
-    <t>xlsxBool</t>
-  </si>
-  <si>
-    <t>[onshow.x_bt;ope=xlsxBool]</t>
-  </si>
-  <si>
-    <t>xlsxDate</t>
-  </si>
-  <si>
-    <t>[onshow.x_dt;ope=xlsxDate]</t>
-  </si>
-  <si>
     <t>When you put a TBS field into a cell, then by default Excel assumes the cell has a string content and will not use the format you expect for the cell.</t>
   </si>
   <si>
     <t>But you can change the type of data in a cell using parameter « ope ». Supported types are listed in the examples below.</t>
   </si>
   <si>
-    <t>[onshow.x_num;ope=xlsxNum]</t>
-  </si>
-  <si>
     <t>* You cannot change picture using "ope=changepic". This is because drawing information are not saved directly in the sheet.</t>
   </si>
   <si>
@@ -193,9 +178,6 @@
   </si>
   <si>
     <t>Score</t>
-  </si>
-  <si>
-    <t>[a.score;ope=xlsxNum]</t>
   </si>
   <si>
     <t>First Name:</t>
@@ -295,9 +277,6 @@
     <t>[a.firstname;block=tbs:row]</t>
   </si>
   <si>
-    <t>[cell2.score;block=tbs:cell;ope=xlsxNum]</t>
-  </si>
-  <si>
     <t>Email [cell1.val;block=tbs:cell]</t>
   </si>
   <si>
@@ -320,6 +299,36 @@
   </si>
   <si>
     <t>Delete a sheet</t>
+  </si>
+  <si>
+    <t>[cell2.score;block=tbs:cell;ope=tbs:num]</t>
+  </si>
+  <si>
+    <t>tbs:num</t>
+  </si>
+  <si>
+    <t>tbs:bool</t>
+  </si>
+  <si>
+    <t>tbs:date</t>
+  </si>
+  <si>
+    <t>[onshow.x_dt;ope=tbs:date]</t>
+  </si>
+  <si>
+    <t>[onshow.x_bt;ope=tbs:bool]</t>
+  </si>
+  <si>
+    <t>[onshow.x_num;ope=tbs:num]</t>
+  </si>
+  <si>
+    <t>[a.score;ope=tbs:num]</t>
+  </si>
+  <si>
+    <t>And this named cell too.</t>
+  </si>
+  <si>
+    <t>Score again</t>
   </si>
 </sst>
 </file>
@@ -600,11 +609,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="54892800"/>
-        <c:axId val="80426112"/>
+        <c:axId val="81547648"/>
+        <c:axId val="81549184"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="54892800"/>
+        <c:axId val="81547648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -613,7 +622,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80426112"/>
+        <c:crossAx val="81549184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -621,7 +630,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="80426112"/>
+        <c:axId val="81549184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -632,7 +641,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="54892800"/>
+        <c:crossAx val="81547648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1076,36 +1085,36 @@
     </row>
     <row r="12" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="2:8" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B17" s="17" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="H17" s="17" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D18" s="13"/>
       <c r="E18" s="14" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="F18" s="15">
         <f>SUM(F20:F2005)</f>
@@ -1123,15 +1132,15 @@
         <v>8</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>9</v>
@@ -1140,56 +1149,56 @@
         <v>10</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C21" s="13"/>
       <c r="D21" s="16" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="E21" s="15">
-        <f ca="1">SUM( E20       : INDIRECT(ADDRESS(ROW()-1,COLUMN())) )</f>
+        <f ca="1">SUM( E20         : INDIRECT(ADDRESS(ROW()-1,COLUMN())) )</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="2:8" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B23" s="17" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="2:8" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B28" s="17" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
@@ -1208,10 +1217,10 @@
         <v>15</v>
       </c>
       <c r="C34" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>25</v>
+        <v>56</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
@@ -1219,10 +1228,10 @@
         <v>16</v>
       </c>
       <c r="C35" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
       <c r="D35" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
@@ -1230,10 +1239,10 @@
         <v>17</v>
       </c>
       <c r="C36" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1259,22 +1268,22 @@
   <sheetData>
     <row r="2" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B2" s="17" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
@@ -1285,43 +1294,43 @@
         <v>7</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B16" s="17" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1345,7 +1354,7 @@
   <sheetData>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1355,7 +1364,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:B4"/>
+  <dimension ref="B2:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1363,12 +1372,17 @@
   <sheetData>
     <row r="2" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B2" s="17" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>39</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
OpenTBS 1.9.1 beta - debug parameter unique
</commit_message>
<xml_diff>
--- a/demo/demo_ms_excel.xlsx
+++ b/demo/demo_ms_excel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="17400" windowHeight="11955"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="17400" windowHeight="11955" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Examples part 1" sheetId="1" r:id="rId1"/>
@@ -609,11 +609,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="81547648"/>
-        <c:axId val="81549184"/>
+        <c:axId val="31805824"/>
+        <c:axId val="31807360"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="81547648"/>
+        <c:axId val="31805824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -622,7 +622,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81549184"/>
+        <c:crossAx val="31807360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -630,7 +630,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="81549184"/>
+        <c:axId val="31807360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -641,7 +641,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81547648"/>
+        <c:crossAx val="31805824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -715,7 +715,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Image 1" descr="[onshow.x_picture;ope=changepic;tagpos=inside;adjust=inside]"/>
+        <xdr:cNvPr id="2" name="Image 1" descr="[onshow.x_picture;ope=changepic;tagpos=inside;adjust=inside;unique]"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1036,7 +1036,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1161,7 +1161,7 @@
         <v>35</v>
       </c>
       <c r="E21" s="15">
-        <f ca="1">SUM( E20         : INDIRECT(ADDRESS(ROW()-1,COLUMN())) )</f>
+        <f ca="1">SUM( E20          : INDIRECT(ADDRESS(ROW()-1,COLUMN())) )</f>
         <v>0</v>
       </c>
     </row>
@@ -1258,7 +1258,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
OpenTBS 1.9.1-beta-2014-07-22 : credit features
</commit_message>
<xml_diff>
--- a/demo/demo_ms_excel.xlsx
+++ b/demo/demo_ms_excel.xlsx
@@ -556,7 +556,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -609,11 +608,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="31805824"/>
-        <c:axId val="31807360"/>
+        <c:axId val="82989440"/>
+        <c:axId val="82990976"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="31805824"/>
+        <c:axId val="82989440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -622,7 +621,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="31807360"/>
+        <c:crossAx val="82990976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -630,7 +629,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="31807360"/>
+        <c:axId val="82990976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -641,14 +640,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="31805824"/>
+        <c:crossAx val="82989440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1161,7 +1159,7 @@
         <v>35</v>
       </c>
       <c r="E21" s="15">
-        <f ca="1">SUM( E20          : INDIRECT(ADDRESS(ROW()-1,COLUMN())) )</f>
+        <f ca="1">SUM( E20           : INDIRECT(ADDRESS(ROW()-1,COLUMN())) )</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
OpenTBS version 1.9.12-beta : can merge charts ins xlsx + example
</commit_message>
<xml_diff>
--- a/demo/demo_ms_excel.xlsx
+++ b/demo/demo_ms_excel.xlsx
@@ -4,16 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="17400" windowHeight="11955" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="17400" windowHeight="11955"/>
   </bookViews>
   <sheets>
-    <sheet name="Examples part 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Examples part 2" sheetId="2" r:id="rId2"/>
-    <sheet name="Display me" sheetId="4" state="hidden" r:id="rId3"/>
-    <sheet name="Delete me" sheetId="3" r:id="rId4"/>
+    <sheet name="Cells and rows" sheetId="1" r:id="rId1"/>
+    <sheet name="Dynamic columns" sheetId="2" r:id="rId2"/>
+    <sheet name="Charts" sheetId="6" r:id="rId3"/>
+    <sheet name="Pictures" sheetId="5" r:id="rId4"/>
+    <sheet name="Sheet to show" sheetId="4" state="hidden" r:id="rId5"/>
+    <sheet name="Sheet to delete" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="the_named_cell">'Delete me'!$B$6</definedName>
+    <definedName name="the_named_cell">'Sheet to delete'!$B$6</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -81,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="71">
   <si>
     <t>PHP version : [onshow..cst.PHP_VERSION]</t>
   </si>
@@ -181,9 +183,6 @@
   </si>
   <si>
     <t>First Name:</t>
-  </si>
-  <si>
-    <t>[cell1.firstname;block=c]</t>
   </si>
   <si>
     <t>[b2.firstname;block=row]</t>
@@ -289,9 +288,6 @@
     <t>Change the type data in a cell</t>
   </si>
   <si>
-    <t>Chart based on dynamic contents</t>
-  </si>
-  <si>
     <t>Dynamic columns</t>
   </si>
   <si>
@@ -328,7 +324,46 @@
     <t>And this named cell too.</t>
   </si>
   <si>
-    <t>Score again</t>
+    <t>[cell1.firstname;block=tbs:cell]</t>
+  </si>
+  <si>
+    <t>Visits</t>
+  </si>
+  <si>
+    <t>[a.visits;ope=tbs:num]</t>
+  </si>
+  <si>
+    <t>Chart with embedded data</t>
+  </si>
+  <si>
+    <t>Chart with linked data</t>
+  </si>
+  <si>
+    <t>When you merge the linked data (the table) then the chart is updated.</t>
+  </si>
+  <si>
+    <t>Victories</t>
+  </si>
+  <si>
+    <t>[b.team;block=tbs:row]</t>
+  </si>
+  <si>
+    <t>[b.victories;ope=tbs:num]</t>
+  </si>
+  <si>
+    <t>And the merged data can push cells placed under.</t>
+  </si>
+  <si>
+    <t>You can also marge data that is embedded with the chart.</t>
+  </si>
+  <si>
+    <t>Unfortunately, this solution needs to have a template with TBS fields instead of illustrating data.</t>
+  </si>
+  <si>
+    <t>This is easier for building the template.</t>
+  </si>
+  <si>
+    <t>Select a series in the chart and its embedded data apears in the formula bar.</t>
   </si>
 </sst>
 </file>
@@ -556,6 +591,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -569,30 +605,35 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Score of the team</c:v>
+            <c:strRef>
+              <c:f>Charts!$H$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Victories</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Examples part 1'!$C$20:$C$24</c:f>
+              <c:f>Charts!$H$5:$H$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>[a.name]</c:v>
+                  <c:v>[b.team;block=tbs:row]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Examples part 1'!$E$20:$E$23</c:f>
+              <c:f>Charts!$I$5:$I$9</c:f>
               <c:numCache>
-                <c:formatCode>#,##0.0</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0" formatCode="#,##0.0">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -608,11 +649,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="82989440"/>
-        <c:axId val="82990976"/>
+        <c:axId val="30263552"/>
+        <c:axId val="30801920"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="82989440"/>
+        <c:axId val="30263552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -621,7 +662,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82990976"/>
+        <c:crossAx val="30801920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -629,7 +670,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82990976"/>
+        <c:axId val="30801920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -640,15 +681,137 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82989440"/>
+        <c:crossAx val="30263552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
-    </c:legend>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Members by category</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="4"/>
+              <c:pt idx="0">
+                <c:v>Newbies</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>Padawan</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>Regular</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>Master</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="4"/>
+              <c:pt idx="0">
+                <c:v>10</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>26</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>45</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>7</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="124172160"/>
+        <c:axId val="124173696"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="124172160"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="124173696"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="124173696"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="124172160"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -665,21 +828,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>19049</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>28574</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>752475</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>161924</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Graphique 1"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -688,6 +853,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>133351</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Graphique 2" descr="The title of the chart is used to merged data from the PHP side." title="chart_members_by_category"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -702,13 +899,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>914400</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>663833</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>140044</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -732,7 +929,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5543550" y="2847975"/>
+          <a:off x="5543550" y="2857500"/>
           <a:ext cx="1130558" cy="1511644"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1032,9 +1229,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H36"/>
+  <dimension ref="B2:F36"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1101,25 +1298,22 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="2:8" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B17" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="H17" s="17" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D18" s="13"/>
       <c r="E18" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F18" s="15">
         <f>SUM(F20:F2005)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
         <v>6</v>
       </c>
@@ -1133,12 +1327,12 @@
         <v>24</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>9</v>
@@ -1147,54 +1341,54 @@
         <v>10</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C21" s="13"/>
       <c r="D21" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E21" s="15">
-        <f ca="1">SUM( E20           : INDIRECT(ADDRESS(ROW()-1,COLUMN())) )</f>
+        <f ca="1">SUM( E20            : INDIRECT(ADDRESS(ROW()-1,COLUMN())) )</f>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:8" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B23" s="17" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8" ht="16.5" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B28" s="17" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
         <v>19</v>
       </c>
@@ -1215,10 +1409,10 @@
         <v>15</v>
       </c>
       <c r="C34" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
@@ -1226,10 +1420,10 @@
         <v>16</v>
       </c>
       <c r="C35" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D35" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
@@ -1237,18 +1431,17 @@
         <v>17</v>
       </c>
       <c r="C36" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1256,7 +1449,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1266,22 +1461,22 @@
   <sheetData>
     <row r="2" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B2" s="17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
@@ -1292,54 +1487,166 @@
         <v>7</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>28</v>
-      </c>
       <c r="D9" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B16" s="17" t="s">
-        <v>48</v>
-      </c>
+      <c r="B16" s="17"/>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="4" t="s">
-        <v>37</v>
-      </c>
+      <c r="B18" s="4"/>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="4" t="s">
-        <v>38</v>
-      </c>
+      <c r="B19" s="4"/>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="4" t="s">
-        <v>39</v>
-      </c>
+      <c r="B20" s="4"/>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="4" t="s">
-        <v>36</v>
-      </c>
+      <c r="B21" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:K25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.140625" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="10" max="10" width="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B2" s="17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B3" s="17"/>
+      <c r="H3" t="s">
+        <v>63</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H5" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K6" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B21" s="17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H23" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H24" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H25" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.140625" customWidth="1"/>
+    <col min="4" max="6" width="20.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B3" s="17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -1352,7 +1659,7 @@
   <sheetData>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1360,7 +1667,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:B6"/>
   <sheetViews>
@@ -1370,17 +1677,17 @@
   <sheetData>
     <row r="2" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B2" s="17" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
improve demo with charts
</commit_message>
<xml_diff>
--- a/demo/demo_ms_excel.xlsx
+++ b/demo/demo_ms_excel.xlsx
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="72">
   <si>
     <t>PHP version : [onshow..cst.PHP_VERSION]</t>
   </si>
@@ -333,12 +333,6 @@
     <t>[a.visits;ope=tbs:num]</t>
   </si>
   <si>
-    <t>Chart with embedded data</t>
-  </si>
-  <si>
-    <t>Chart with linked data</t>
-  </si>
-  <si>
     <t>When you merge the linked data (the table) then the chart is updated.</t>
   </si>
   <si>
@@ -354,16 +348,25 @@
     <t>And the merged data can push cells placed under.</t>
   </si>
   <si>
-    <t>You can also marge data that is embedded with the chart.</t>
-  </si>
-  <si>
     <t>Unfortunately, this solution needs to have a template with TBS fields instead of illustrating data.</t>
   </si>
   <si>
-    <t>This is easier for building the template.</t>
-  </si>
-  <si>
-    <t>Select a series in the chart and its embedded data apears in the formula bar.</t>
+    <t>↕ texts separated with 1 line in the template</t>
+  </si>
+  <si>
+    <t>OpenTBS can also merge data that is embedded within the chart.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You can convert a chart linked to ranges into an unlinked chart by selecting the </t>
+  </si>
+  <si>
+    <t>The references in the formula of the series are thus converted into literal values.</t>
+  </si>
+  <si>
+    <t>This is easier for building the chart in the template since you can tune the chard design with a sample of data.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    series in the chart, then select the formula bar, and press F9.</t>
   </si>
 </sst>
 </file>
@@ -375,7 +378,7 @@
     <numFmt numFmtId="165" formatCode="dd\ mmmm\ yyyy"/>
     <numFmt numFmtId="166" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -463,6 +466,13 @@
       <family val="1"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="2" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -527,7 +537,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -556,6 +566,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -591,6 +602,29 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600">
+                <a:solidFill>
+                  <a:schemeClr val="tx2">
+                    <a:lumMod val="60000"/>
+                    <a:lumOff val="40000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mj-lt"/>
+              </a:rPr>
+              <a:t>Chart with linked data</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
     </c:title>
@@ -606,7 +640,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Charts!$H$3</c:f>
+              <c:f>Charts!$H$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -618,7 +652,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Charts!$H$5:$H$9</c:f>
+              <c:f>Charts!$H$4:$H$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -629,7 +663,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Charts!$I$5:$I$9</c:f>
+              <c:f>Charts!$I$4:$I$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -649,11 +683,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="30263552"/>
-        <c:axId val="30801920"/>
+        <c:axId val="175826048"/>
+        <c:axId val="175827584"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="30263552"/>
+        <c:axId val="175826048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -662,7 +696,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="30801920"/>
+        <c:crossAx val="175827584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -670,7 +704,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="30801920"/>
+        <c:axId val="175827584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -681,7 +715,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="30263552"/>
+        <c:crossAx val="175826048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -713,8 +747,35 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.14519923951661151"/>
+          <c:y val="3.9473684210526314E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -727,7 +788,7 @@
           <c:idx val="1"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Members by category</c:v>
+            <c:v>Chart with unliked embedded data</c:v>
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:cat>
@@ -775,11 +836,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="124172160"/>
-        <c:axId val="124173696"/>
+        <c:axId val="176134400"/>
+        <c:axId val="126332928"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="124172160"/>
+        <c:axId val="176134400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -788,7 +849,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="124173696"/>
+        <c:crossAx val="126332928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -796,7 +857,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="124173696"/>
+        <c:axId val="126332928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -807,7 +868,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="124172160"/>
+        <c:crossAx val="176134400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -828,16 +889,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>28574</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>342899</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -861,15 +922,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>133351</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:colOff>152401</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -888,6 +949,54 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>752475</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>676276</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Connecteur droit avec flèche 4"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="4752975" y="590550"/>
+          <a:ext cx="685801" cy="333375"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:headEnd type="oval"/>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1353,7 +1462,7 @@
         <v>34</v>
       </c>
       <c r="E21" s="15">
-        <f ca="1">SUM( E20            : INDIRECT(ADDRESS(ROW()-1,COLUMN())) )</f>
+        <f ca="1">SUM( E20             : INDIRECT(ADDRESS(ROW()-1,COLUMN())) )</f>
         <v>0</v>
       </c>
     </row>
@@ -1449,9 +1558,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1525,7 +1632,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:K25"/>
+  <dimension ref="B1:L27"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1537,63 +1644,73 @@
     <col min="10" max="10" width="4" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B1" s="17"/>
+    </row>
     <row r="2" spans="2:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="17"/>
+      <c r="H2" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="3" spans="2:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B3" s="17"/>
-      <c r="H3" t="s">
+      <c r="K2" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H4" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="I4" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="K3" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="H4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K4" s="4" t="s">
+      <c r="K4" s="18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K5" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B20" s="17"/>
+      <c r="H20" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="H21" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="H23" s="4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="H5" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="K6" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B21" s="17" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H23" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="H24" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="H25" s="4" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H25" s="4" t="s">
-        <v>70</v>
-      </c>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L27" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[demo] update XLSX and ODS templates
</commit_message>
<xml_diff>
--- a/demo/demo_ms_excel.xlsx
+++ b/demo/demo_ms_excel.xlsx
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="73">
   <si>
     <t>PHP version : [onshow..cst.PHP_VERSION]</t>
   </si>
@@ -183,9 +183,6 @@
   </si>
   <si>
     <t>First Name:</t>
-  </si>
-  <si>
-    <t>[b2.firstname;block=row]</t>
   </si>
   <si>
     <t>[b2.name]</t>
@@ -270,15 +267,9 @@
     <t>the description (or title) of the picture item, and use</t>
   </si>
   <si>
-    <t>[b2.email_[cell2.val;block=tbs:cell]]</t>
-  </si>
-  <si>
     <t>[a.firstname;block=tbs:row]</t>
   </si>
   <si>
-    <t>Email [cell1.val;block=tbs:cell]</t>
-  </si>
-  <si>
     <t>Merging data with rows</t>
   </si>
   <si>
@@ -297,9 +288,6 @@
     <t>Delete a sheet</t>
   </si>
   <si>
-    <t>[cell2.score;block=tbs:cell;ope=tbs:num]</t>
-  </si>
-  <si>
     <t>tbs:num</t>
   </si>
   <si>
@@ -324,9 +312,6 @@
     <t>And this named cell too.</t>
   </si>
   <si>
-    <t>[cell1.firstname;block=tbs:cell]</t>
-  </si>
-  <si>
     <t>Visits</t>
   </si>
   <si>
@@ -339,12 +324,6 @@
     <t>Victories</t>
   </si>
   <si>
-    <t>[b.team;block=tbs:row]</t>
-  </si>
-  <si>
-    <t>[b.victories;ope=tbs:num]</t>
-  </si>
-  <si>
     <t>And the merged data can push cells placed under.</t>
   </si>
   <si>
@@ -367,6 +346,30 @@
   </si>
   <si>
     <t xml:space="preserve">    series in the chart, then select the formula bar, and press F9.</t>
+  </si>
+  <si>
+    <t>Show or hide a sheet</t>
+  </si>
+  <si>
+    <t>[c1.firstname;block=tbs:cell]</t>
+  </si>
+  <si>
+    <t>[c2.score;block=tbs:cell;ope=tbs:num]</t>
+  </si>
+  <si>
+    <t>[b2.firstname;block=tbs:row]</t>
+  </si>
+  <si>
+    <t>Email [dc1.val;block=tbs:cell]</t>
+  </si>
+  <si>
+    <t>[b2.email_[dc2.val;block=tbs:cell]]</t>
+  </si>
+  <si>
+    <t>[ch.team;block=tbs:row]</t>
+  </si>
+  <si>
+    <t>[ch.victories;ope=tbs:num]</t>
   </si>
 </sst>
 </file>
@@ -549,12 +552,6 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -567,6 +564,12 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -656,7 +659,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>[b.team;block=tbs:row]</c:v>
+                  <c:v>[ch.team;block=tbs:row]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -683,11 +686,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="175826048"/>
-        <c:axId val="175827584"/>
+        <c:axId val="150029056"/>
+        <c:axId val="150030592"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="175826048"/>
+        <c:axId val="150029056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -696,7 +699,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="175827584"/>
+        <c:crossAx val="150030592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -704,7 +707,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="175827584"/>
+        <c:axId val="150030592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -715,7 +718,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="175826048"/>
+        <c:crossAx val="150029056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -836,11 +839,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="176134400"/>
-        <c:axId val="126332928"/>
+        <c:axId val="150050688"/>
+        <c:axId val="150052224"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="176134400"/>
+        <c:axId val="150050688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -849,7 +852,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="126332928"/>
+        <c:crossAx val="150052224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -857,7 +860,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="126332928"/>
+        <c:axId val="150052224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -868,7 +871,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="176134400"/>
+        <c:crossAx val="150050688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1408,16 +1411,16 @@
       </c>
     </row>
     <row r="17" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B17" s="17" t="s">
-        <v>42</v>
+      <c r="B17" s="15" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D18" s="13"/>
-      <c r="E18" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="F18" s="15">
+      <c r="D18" s="11"/>
+      <c r="E18" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" s="13">
         <f>SUM(F20:F2005)</f>
         <v>0</v>
       </c>
@@ -1436,12 +1439,12 @@
         <v>24</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>9</v>
@@ -1450,46 +1453,46 @@
         <v>10</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C21" s="13"/>
-      <c r="D21" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="E21" s="15">
-        <f ca="1">SUM( E20             : INDIRECT(ADDRESS(ROW()-1,COLUMN())) )</f>
+      <c r="C21" s="11"/>
+      <c r="D21" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E21" s="13">
+        <f ca="1">SUM( E20              : INDIRECT(ADDRESS(ROW()-1,COLUMN())) )</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B23" s="17" t="s">
-        <v>43</v>
+      <c r="B23" s="15" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="9" t="s">
-        <v>57</v>
+      <c r="C25" s="17" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="10" t="s">
-        <v>48</v>
+      <c r="C26" s="18" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="28" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B28" s="17" t="s">
-        <v>44</v>
+      <c r="B28" s="15" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
@@ -1518,10 +1521,10 @@
         <v>15</v>
       </c>
       <c r="C34" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
@@ -1529,10 +1532,10 @@
         <v>16</v>
       </c>
       <c r="C35" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D35" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
@@ -1540,10 +1543,10 @@
         <v>17</v>
       </c>
       <c r="C36" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1567,23 +1570,23 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B2" s="17" t="s">
-        <v>45</v>
+      <c r="B2" s="15" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
@@ -1593,23 +1596,23 @@
       <c r="C8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="12" t="s">
-        <v>41</v>
+      <c r="D8" s="10" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>39</v>
+      <c r="D9" s="9" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B16" s="17"/>
+      <c r="B16" s="15"/>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="4"/>
@@ -1645,15 +1648,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B1" s="17"/>
+      <c r="B1" s="15"/>
     </row>
     <row r="2" spans="2:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B2" s="17"/>
+      <c r="B2" s="15"/>
       <c r="H2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
@@ -1664,49 +1667,49 @@
         <v>24</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="H4" s="3" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="K4" s="18" t="s">
-        <v>66</v>
+        <v>72</v>
+      </c>
+      <c r="K4" s="16" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="K5" s="4" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="2:12" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B20" s="17"/>
+      <c r="B20" s="15"/>
       <c r="H20" s="4" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="H21" s="4" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="H23" s="4" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="H24" s="4" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.25">
       <c r="H25" s="4" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.25">
@@ -1732,28 +1735,28 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B3" s="17" t="s">
-        <v>46</v>
+      <c r="B3" s="15" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1768,15 +1771,20 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="B3"/>
+  <dimension ref="B2:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>32</v>
+    <row r="2" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B2" s="15" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1793,18 +1801,18 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B2" s="17" t="s">
-        <v>47</v>
+      <c r="B2" s="15" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>